<commit_message>
fixed bug when rows(objects) deleted or added then the range references were not updated accordingly
</commit_message>
<xml_diff>
--- a/SpreadsheetDatalayer/SpreadsheetDataLayer.NUnit/App_Data/Equipment.xlsx
+++ b/SpreadsheetDatalayer/SpreadsheetDataLayer.NUnit/App_Data/Equipment.xlsx
@@ -999,253 +999,461 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>7</v>
-      </c>
-      <c r="G3">
-        <v>8</v>
-      </c>
-      <c r="H3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <v>8</v>
-      </c>
-      <c r="G6">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>8</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8">
-        <v>9</v>
-      </c>
-      <c r="E8">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9">
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <v>8</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:dimension ref="A1:H17"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:8">
+      <x:c r="A1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="G1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:8">
+      <x:c r="A2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D2">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E2">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F2">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="G2">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="H2">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:8">
+      <x:c r="A3" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B3" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D3">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="E3">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F3">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="G3">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H3">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:8">
+      <x:c r="A4" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C4" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D4">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E4">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F4">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="G4">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H4">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:8">
+      <x:c r="A5" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B5" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D5">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E5">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F5">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="G5">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H5">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:8">
+      <x:c r="A6" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B6" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C6" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D6">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E6">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="F6">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="G6">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H6">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:8">
+      <x:c r="A7" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B7" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C7" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D7">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E7">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F7">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G7">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H7">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:8">
+      <x:c r="A8" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B8" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C8" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D8">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E8">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F8">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G8">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H8">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:8">
+      <x:c r="A9" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B9" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C9" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D9">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E9">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F9">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G9">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="H9">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:8">
+      <x:c r="A10" t="str">
+        <x:v>Equip-101</x:v>
+      </x:c>
+      <x:c r="B10" t="str">
+        <x:v>PT-4</x:v>
+      </x:c>
+      <x:c r="C10" t="str">
+        <x:v>PDT-9</x:v>
+      </x:c>
+      <x:c r="D10" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E10" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F10" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="G10" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H10" t="n">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:8">
+      <x:c r="A11" t="str">
+        <x:v>Equip-102</x:v>
+      </x:c>
+      <x:c r="B11" t="str">
+        <x:v>PT-9</x:v>
+      </x:c>
+      <x:c r="C11" t="str">
+        <x:v>PDT-5</x:v>
+      </x:c>
+      <x:c r="D11" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E11" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F11" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="G11" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="H11" t="n">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:8">
+      <x:c r="A12" t="str">
+        <x:v>Equip-103</x:v>
+      </x:c>
+      <x:c r="B12" t="str">
+        <x:v>PT-9</x:v>
+      </x:c>
+      <x:c r="C12" t="str">
+        <x:v>PDT-6</x:v>
+      </x:c>
+      <x:c r="D12" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="E12" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F12" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="G12" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H12" t="n">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:8">
+      <x:c r="A13" t="str">
+        <x:v>Equip-104</x:v>
+      </x:c>
+      <x:c r="B13" t="str">
+        <x:v>PT-9</x:v>
+      </x:c>
+      <x:c r="C13" t="str">
+        <x:v>PDT-2</x:v>
+      </x:c>
+      <x:c r="D13" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E13" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F13" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="G13" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H13" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:8">
+      <x:c r="A14" t="str">
+        <x:v>Equip-105</x:v>
+      </x:c>
+      <x:c r="B14" t="str">
+        <x:v>PT-3</x:v>
+      </x:c>
+      <x:c r="C14" t="str">
+        <x:v>PDT-8</x:v>
+      </x:c>
+      <x:c r="D14" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E14" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F14" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G14" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H14" t="n">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:8">
+      <x:c r="A15" t="str">
+        <x:v>Equip-106</x:v>
+      </x:c>
+      <x:c r="B15" t="str">
+        <x:v>PT-3</x:v>
+      </x:c>
+      <x:c r="C15" t="str">
+        <x:v>PDT-9</x:v>
+      </x:c>
+      <x:c r="D15" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E15" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F15" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="G15" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H15" t="n">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:8">
+      <x:c r="A16" t="str">
+        <x:v>Equip-107</x:v>
+      </x:c>
+      <x:c r="B16" t="str">
+        <x:v>PT-7</x:v>
+      </x:c>
+      <x:c r="C16" t="str">
+        <x:v>PDT-4</x:v>
+      </x:c>
+      <x:c r="D16" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E16" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F16" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G16" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H16" t="n">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:8">
+      <x:c r="A17" t="str">
+        <x:v>Equip-108</x:v>
+      </x:c>
+      <x:c r="B17" t="str">
+        <x:v>PT-8</x:v>
+      </x:c>
+      <x:c r="C17" t="str">
+        <x:v>PDT-9</x:v>
+      </x:c>
+      <x:c r="D17" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E17" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F17" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G17" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H17" t="n">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
modified spreadsheet datalayer to work with new directory
</commit_message>
<xml_diff>
--- a/SpreadsheetDatalayer/SpreadsheetDataLayer.NUnit/App_Data/Equipment.xlsx
+++ b/SpreadsheetDatalayer/SpreadsheetDataLayer.NUnit/App_Data/Equipment.xlsx
@@ -1248,25 +1248,25 @@
         <x:v>Equip-101</x:v>
       </x:c>
       <x:c r="B10" t="str">
-        <x:v>PT-4</x:v>
+        <x:v>PT-8</x:v>
       </x:c>
       <x:c r="C10" t="str">
-        <x:v>PDT-9</x:v>
+        <x:v>PDT-6</x:v>
       </x:c>
       <x:c r="D10" t="n">
-        <x:v>9</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E10" t="n">
-        <x:v>9</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="F10" t="n">
-        <x:v>7</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="G10" t="n">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="H10" t="n">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -1274,25 +1274,25 @@
         <x:v>Equip-102</x:v>
       </x:c>
       <x:c r="B11" t="str">
-        <x:v>PT-9</x:v>
+        <x:v>PT-7</x:v>
       </x:c>
       <x:c r="C11" t="str">
-        <x:v>PDT-5</x:v>
+        <x:v>PDT-6</x:v>
       </x:c>
       <x:c r="D11" t="n">
         <x:v>4</x:v>
       </x:c>
       <x:c r="E11" t="n">
-        <x:v>9</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="F11" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="G11" t="n">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="G11" t="n">
-        <x:v>7</x:v>
-      </x:c>
       <x:c r="H11" t="n">
-        <x:v>7</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -1300,25 +1300,25 @@
         <x:v>Equip-103</x:v>
       </x:c>
       <x:c r="B12" t="str">
-        <x:v>PT-9</x:v>
+        <x:v>PT-6</x:v>
       </x:c>
       <x:c r="C12" t="str">
-        <x:v>PDT-6</x:v>
+        <x:v>PDT-4</x:v>
       </x:c>
       <x:c r="D12" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E12" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="F12" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="G12" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="E12" t="n">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="F12" t="n">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="G12" t="n">
+      <x:c r="H12" t="n">
         <x:v>4</x:v>
-      </x:c>
-      <x:c r="H12" t="n">
-        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -1326,25 +1326,25 @@
         <x:v>Equip-104</x:v>
       </x:c>
       <x:c r="B13" t="str">
-        <x:v>PT-9</x:v>
+        <x:v>PT-7</x:v>
       </x:c>
       <x:c r="C13" t="str">
         <x:v>PDT-2</x:v>
       </x:c>
       <x:c r="D13" t="n">
-        <x:v>7</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E13" t="n">
-        <x:v>4</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F13" t="n">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="G13" t="n">
         <x:v>6</x:v>
       </x:c>
       <x:c r="H13" t="n">
-        <x:v>3</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -1352,25 +1352,25 @@
         <x:v>Equip-105</x:v>
       </x:c>
       <x:c r="B14" t="str">
-        <x:v>PT-3</x:v>
+        <x:v>PT-6</x:v>
       </x:c>
       <x:c r="C14" t="str">
-        <x:v>PDT-8</x:v>
+        <x:v>PDT-5</x:v>
       </x:c>
       <x:c r="D14" t="n">
         <x:v>6</x:v>
       </x:c>
       <x:c r="E14" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F14" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="G14" t="n">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G14" t="n">
-        <x:v>9</x:v>
-      </x:c>
       <x:c r="H14" t="n">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1378,25 +1378,25 @@
         <x:v>Equip-106</x:v>
       </x:c>
       <x:c r="B15" t="str">
-        <x:v>PT-3</x:v>
+        <x:v>PT-4</x:v>
       </x:c>
       <x:c r="C15" t="str">
-        <x:v>PDT-9</x:v>
+        <x:v>PDT-6</x:v>
       </x:c>
       <x:c r="D15" t="n">
-        <x:v>9</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E15" t="n">
-        <x:v>2</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="F15" t="n">
-        <x:v>6</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="G15" t="n">
-        <x:v>9</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="H15" t="n">
-        <x:v>9</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1404,25 +1404,25 @@
         <x:v>Equip-107</x:v>
       </x:c>
       <x:c r="B16" t="str">
-        <x:v>PT-7</x:v>
+        <x:v>PT-2</x:v>
       </x:c>
       <x:c r="C16" t="str">
-        <x:v>PDT-4</x:v>
+        <x:v>PDT-7</x:v>
       </x:c>
       <x:c r="D16" t="n">
         <x:v>7</x:v>
       </x:c>
       <x:c r="E16" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F16" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="G16" t="n">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="F16" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="G16" t="n">
-        <x:v>2</x:v>
-      </x:c>
       <x:c r="H16" t="n">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1430,25 +1430,25 @@
         <x:v>Equip-108</x:v>
       </x:c>
       <x:c r="B17" t="str">
-        <x:v>PT-8</x:v>
+        <x:v>PT-5</x:v>
       </x:c>
       <x:c r="C17" t="str">
-        <x:v>PDT-9</x:v>
+        <x:v>PDT-6</x:v>
       </x:c>
       <x:c r="D17" t="n">
-        <x:v>9</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E17" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="F17" t="n">
         <x:v>5</x:v>
       </x:c>
       <x:c r="G17" t="n">
-        <x:v>8</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H17" t="n">
-        <x:v>4</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>